<commit_message>
ajout description contact page
</commit_message>
<xml_diff>
--- a/sources/Modèle-audit-SEO.xlsx
+++ b/sources/Modèle-audit-SEO.xlsx
@@ -168,6 +168,39 @@
   <si>
     <t>https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist#text_equivalents</t>
   </si>
+  <si>
+    <t>FichierJ</t>
+  </si>
+  <si>
+    <t>Fichier JS et CSS pas optimisés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les fichiers peuvent être compresser pour diminuer la vitesse de chargement du site </t>
+  </si>
+  <si>
+    <t>Mot clés pas optimisés, doublon de mots, et hors sujet Div “keyword” invisible dans le body pour le réferencement qui ne sert à rien</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mot clés pas optimisés (doublon de mots, et hors sujet.)          Div “keyword” invisible dans le body pour le réferencement qui ne sert à rien</t>
+  </si>
+  <si>
+    <t>Pas de titre et de description dans les meta du site  langue du site parametrée sur “Default” ce qui ne sert à rien ici</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toujours rendre le texte lisible pour les bots d'indexation, donc ne pas afficher un texte sur une image car il ne sera pas pris en compte pour l'indexation du site </t>
+  </si>
+  <si>
+    <t>Metadonnés du site</t>
+  </si>
+  <si>
+    <t>Opacité des  textes</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/search/docs/advanced/crawling/special-tags?hl=fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
@@ -176,7 +209,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -276,6 +309,11 @@
       <name val="Arial"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -325,7 +363,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -419,6 +457,10 @@
       <protection/>
     </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="14" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" applyAlignment="1" applyProtection="1" xfId="0">
+      <alignment wrapText="1" vertical="center" horizontal="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="15" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" applyAlignment="1" applyProtection="1" xfId="0">
       <alignment wrapText="1" vertical="center" horizontal="center"/>
       <protection/>
     </xf>
@@ -501,8 +543,8 @@
   </sheetPr>
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.12890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -510,8 +552,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="48"/>
-    <col collapsed="false" customWidth="1" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29"/>
-    <col collapsed="false" customWidth="1" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="29"/>
+    <col collapsed="false" customWidth="1" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.2188"/>
+    <col collapsed="false" customWidth="1" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="32.1094"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="27.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10.57"/>
@@ -1577,42 +1619,44 @@
       <c r="A2" s="4"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" ht="51">
+    <row r="3" ht="28">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>9</v>
+        <v>56</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" ht="51">
+    <row r="4" ht="42">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="5"/>
+      <c r="C4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F4" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" ht="51">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" ht="28">
       <c r="A5" s="6" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="E5" s="5"/>
     </row>
@@ -1621,7 +1665,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
@@ -1631,7 +1675,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" ht="55">
+    <row r="7" ht="69">
       <c r="A7" s="6" t="s">
         <v>35</v>
       </c>
@@ -1642,7 +1686,7 @@
         <v>19</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>48</v>
@@ -1658,9 +1702,11 @@
       <c r="C8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F8" s="8" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" customHeight="1" ht="42">
@@ -1754,12 +1800,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" display="http://www.seo-hero.tech/"/>
     <hyperlink ref="F12" display="https://support.google.com/webmasters/answer/9128668?hl=fr" r:id="rId2"/>
     <hyperlink ref="F8" display="https://rootsteps.nl/en/blog/deadlinks-on-your-website-and-why-you-should-search-for-them-regularly" r:id="rId3"/>
     <hyperlink ref="F6" display="https://color.a11y.com/Contrast/" r:id="rId4"/>
     <hyperlink ref="F7" display="https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist#text_equivalents" r:id="rId5"/>
     <hyperlink ref="F10" display="https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist#text_equivalents" r:id="rId6"/>
+    <hyperlink ref="F4" display="https://developers.google.com/search/docs/advanced/crawling/special-tags?hl=fr" r:id="rId7"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>